<commit_message>
Added some basic excel reading logic
</commit_message>
<xml_diff>
--- a/etl/sample_files/ExampleFile.xlsx
+++ b/etl/sample_files/ExampleFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Spikes\Python-SCD-ETL\etl\sample_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F18DCD83-FC72-49BD-9381-C8CD2CCDAE2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F92F182C-3790-4798-BEEB-349FC87E18A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37995" yWindow="3885" windowWidth="17430" windowHeight="9585" xr2:uid="{3D8AFFFE-4EB6-46E8-938A-B3657704E572}"/>
+    <workbookView xWindow="5604" yWindow="2772" windowWidth="17436" windowHeight="9588" xr2:uid="{3D8AFFFE-4EB6-46E8-938A-B3657704E572}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,18 +41,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
   <si>
-    <t>Process Date</t>
-  </si>
-  <si>
-    <t>External Reference</t>
-  </si>
-  <si>
-    <t>Client Account</t>
-  </si>
-  <si>
-    <t>Company Name</t>
-  </si>
-  <si>
     <t>Amount</t>
   </si>
   <si>
@@ -156,6 +144,18 @@
   </si>
   <si>
     <t>Pending</t>
+  </si>
+  <si>
+    <t>ProcessDate</t>
+  </si>
+  <si>
+    <t>ClientAccount</t>
+  </si>
+  <si>
+    <t>ExternalReference</t>
+  </si>
+  <si>
+    <t>CompanyName</t>
   </si>
 </sst>
 </file>
@@ -163,8 +163,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
-    <numFmt numFmtId="167" formatCode="&quot;R&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="165" formatCode="&quot;R&quot;#,##0.00"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -217,14 +217,14 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -543,7 +543,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -558,22 +558,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -581,19 +581,19 @@
         <v>44843</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E2" s="5">
         <v>358666.8</v>
       </c>
       <c r="F2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -601,19 +601,19 @@
         <v>44843</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E3" s="5">
         <v>500000</v>
       </c>
       <c r="F3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -621,19 +621,19 @@
         <v>44843</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E4" s="5">
         <v>120000</v>
       </c>
       <c r="F4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -641,19 +641,19 @@
         <v>44843</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E5" s="5">
         <v>50</v>
       </c>
       <c r="F5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -661,16 +661,16 @@
         <v>44843</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -678,19 +678,19 @@
         <v>44843</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E7" s="5">
         <v>356900</v>
       </c>
       <c r="F7" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -698,19 +698,19 @@
         <v>44843</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E8" s="5">
         <v>899000</v>
       </c>
       <c r="F8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -718,19 +718,19 @@
         <v>44843</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E9" s="5">
         <v>2300</v>
       </c>
       <c r="F9" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -738,19 +738,19 @@
         <v>44843</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D10" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E10" s="5">
         <v>230000</v>
       </c>
       <c r="F10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -758,19 +758,19 @@
         <v>44843</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E11" s="5">
         <v>100000</v>
       </c>
       <c r="F11" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Basic excel file processing and ETL
</commit_message>
<xml_diff>
--- a/etl/sample_files/ExampleFile.xlsx
+++ b/etl/sample_files/ExampleFile.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Spikes\Python-SCD-ETL\etl\sample_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Python-SCD-ETL\etl\sample_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F92F182C-3790-4798-BEEB-349FC87E18A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{136461A5-DFEC-4705-B610-695702667628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5604" yWindow="2772" windowWidth="17436" windowHeight="9588" xr2:uid="{3D8AFFFE-4EB6-46E8-938A-B3657704E572}"/>
+    <workbookView xWindow="2352" yWindow="1152" windowWidth="17280" windowHeight="8880" xr2:uid="{3D8AFFFE-4EB6-46E8-938A-B3657704E572}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -146,16 +146,16 @@
     <t>Pending</t>
   </si>
   <si>
-    <t>ProcessDate</t>
-  </si>
-  <si>
-    <t>ClientAccount</t>
-  </si>
-  <si>
-    <t>ExternalReference</t>
-  </si>
-  <si>
-    <t>CompanyName</t>
+    <t>Effective Date</t>
+  </si>
+  <si>
+    <t>Client Account</t>
+  </si>
+  <si>
+    <t>External Reference</t>
+  </si>
+  <si>
+    <t>Company Name</t>
   </si>
 </sst>
 </file>
@@ -543,7 +543,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
+      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Updated to pydantic mappings and refactored file processing
</commit_message>
<xml_diff>
--- a/etl/sample_files/ExampleFile.xlsx
+++ b/etl/sample_files/ExampleFile.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Python-SCD-ETL\etl\sample_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Spikes\Python-SCD-ETL\etl\sample_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{136461A5-DFEC-4705-B610-695702667628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DF82D9B-EE3B-4579-B92C-94C6E04A1CE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2352" yWindow="1152" windowWidth="17280" windowHeight="8880" xr2:uid="{3D8AFFFE-4EB6-46E8-938A-B3657704E572}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3D8AFFFE-4EB6-46E8-938A-B3657704E572}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,9 +44,6 @@
     <t>Amount</t>
   </si>
   <si>
-    <t>Status</t>
-  </si>
-  <si>
     <t>CL-001</t>
   </si>
   <si>
@@ -137,15 +134,6 @@
     <t>Company J</t>
   </si>
   <si>
-    <t>Active</t>
-  </si>
-  <si>
-    <t>Inactive</t>
-  </si>
-  <si>
-    <t>Pending</t>
-  </si>
-  <si>
     <t>Effective Date</t>
   </si>
   <si>
@@ -156,6 +144,18 @@
   </si>
   <si>
     <t>Company Name</t>
+  </si>
+  <si>
+    <t>Term</t>
+  </si>
+  <si>
+    <t>Cash</t>
+  </si>
+  <si>
+    <t>30 Days</t>
+  </si>
+  <si>
+    <t>7 Days</t>
   </si>
 </sst>
 </file>
@@ -543,7 +543,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
+      <selection pane="bottomLeft" activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -558,22 +558,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>1</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -581,19 +581,19 @@
         <v>44843</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E2" s="5">
         <v>358666.8</v>
       </c>
       <c r="F2" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -601,19 +601,19 @@
         <v>44843</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3" s="5">
         <v>500000</v>
       </c>
       <c r="F3" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -621,19 +621,19 @@
         <v>44843</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E4" s="5">
         <v>120000</v>
       </c>
       <c r="F4" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -641,19 +641,19 @@
         <v>44843</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E5" s="5">
         <v>50</v>
       </c>
       <c r="F5" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -661,16 +661,16 @@
         <v>44843</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F6" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -678,19 +678,19 @@
         <v>44843</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E7" s="5">
         <v>356900</v>
       </c>
       <c r="F7" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -698,19 +698,19 @@
         <v>44843</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E8" s="5">
         <v>899000</v>
       </c>
       <c r="F8" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -718,19 +718,19 @@
         <v>44843</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E9" s="5">
         <v>2300</v>
       </c>
       <c r="F9" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -738,19 +738,19 @@
         <v>44843</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E10" s="5">
         <v>230000</v>
       </c>
       <c r="F10" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -758,24 +758,25 @@
         <v>44843</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E11" s="5">
         <v>100000</v>
       </c>
       <c r="F11" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F1" xr:uid="{C99AC18E-6CF0-40F9-A836-EDB33EB766E0}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>